<commit_message>
[強制DM] [add field] scinario_17
</commit_message>
<xml_diff>
--- a/app/seeds/news.xlsx
+++ b/app/seeds/news.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>コレクション定義</t>
     <phoneticPr fontId="1"/>
@@ -274,6 +274,25 @@
     <rPh sb="0" eb="2">
       <t>ハイシンキカン</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>title</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>文字列</t>
+    <rPh sb="0" eb="3">
+      <t>モジレツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイトル</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイトル</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -384,8 +403,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -430,7 +453,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="25">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -441,6 +464,8 @@
     <cellStyle name="ハイパーリンク" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -452,6 +477,8 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="24" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -888,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1070,66 +1097,87 @@
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="5"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="A15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="10" t="s">
+    <row r="18" spans="1:8">
+      <c r="A18" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B18" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C18" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D18" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G18" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="2">
+      <c r="H18" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="2">
         <v>1</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B19" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C19" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D19" s="12">
         <v>41624</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12">
+      <c r="E19" s="12"/>
+      <c r="F19" s="12">
         <v>41624.166666666664</v>
       </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
+      <c r="G19" s="2"/>
+      <c r="H19" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[強制DM] [edit field] scinario_18
</commit_message>
<xml_diff>
--- a/app/seeds/news.xlsx
+++ b/app/seeds/news.xlsx
@@ -918,7 +918,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -926,7 +926,7 @@
     <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" customWidth="1"/>
     <col min="3" max="3" width="32.1640625" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="28.5" customWidth="1"/>
     <col min="6" max="6" width="32.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" customWidth="1"/>
@@ -1023,7 +1023,9 @@
       <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
       <c r="E10" s="6" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
[強制DM] [delete field] scinario_19
</commit_message>
<xml_diff>
--- a/app/seeds/news.xlsx
+++ b/app/seeds/news.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>コレクション定義</t>
     <phoneticPr fontId="1"/>
@@ -274,25 +274,6 @@
     <rPh sb="0" eb="2">
       <t>ハイシンキカン</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>title</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>文字列</t>
-    <rPh sb="0" eb="3">
-      <t>モジレツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイトル</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイトル</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -915,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H17" sqref="H17:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1099,87 +1080,66 @@
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="5"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="5" t="s">
+      <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="10" t="s">
+    <row r="17" spans="1:7">
+      <c r="A17" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H18" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="2">
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="2">
         <v>1</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B18" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C18" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D18" s="12">
         <v>41624</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12">
+      <c r="E18" s="12"/>
+      <c r="F18" s="12">
         <v>41624.166666666664</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="G18" s="2"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[強制DM] [add data] scinario_20
</commit_message>
<xml_diff>
--- a/app/seeds/news.xlsx
+++ b/app/seeds/news.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>コレクション定義</t>
     <phoneticPr fontId="1"/>
@@ -274,6 +274,14 @@
     <rPh sb="0" eb="2">
       <t>ハイシンキカン</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サーバ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>メンテナンスします</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -384,7 +392,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -410,8 +418,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -433,8 +445,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="29">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -447,6 +460,8 @@
     <cellStyle name="ハイパーリンク" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -460,6 +475,8 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="28" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -899,7 +916,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:H18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1133,6 +1150,25 @@
       </c>
       <c r="G18" s="2"/>
     </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="2">
+        <v>2</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="12">
+        <v>41730</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12">
+        <v>41731</v>
+      </c>
+      <c r="G19" s="2"/>
+    </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
[強制DM] [edit data] scinario_21
</commit_message>
<xml_diff>
--- a/app/seeds/news.xlsx
+++ b/app/seeds/news.xlsx
@@ -916,7 +916,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12">
-        <v>41731</v>
+        <v>41730.125</v>
       </c>
       <c r="G19" s="2"/>
     </row>

</xml_diff>

<commit_message>
[強制DM] [delete data] scinario_22
</commit_message>
<xml_diff>
--- a/app/seeds/news.xlsx
+++ b/app/seeds/news.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>コレクション定義</t>
     <phoneticPr fontId="1"/>
@@ -274,14 +274,6 @@
     <rPh sb="0" eb="2">
       <t>ハイシンキカン</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>サーバ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>メンテナンスします</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -423,7 +415,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -445,7 +437,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
@@ -913,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1021,9 +1012,7 @@
       <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
+      <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
         <v>26</v>
       </c>
@@ -1150,32 +1139,13 @@
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="2">
-        <v>2</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="12">
-        <v>41730</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12">
-        <v>41730.125</v>
-      </c>
-      <c r="G19" s="2"/>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[強制DM] [delete data] scinario_22 newのappseed修正
</commit_message>
<xml_diff>
--- a/app/seeds/news.xlsx
+++ b/app/seeds/news.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>コレクション定義</t>
     <phoneticPr fontId="1"/>
@@ -166,16 +166,6 @@
     <t>お知らせID</t>
     <rPh sb="1" eb="2">
       <t>シ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お知らせ期間FROM</t>
-    <rPh sb="1" eb="2">
-      <t>シ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ハイシンキカン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -270,7 +260,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>期間TO</t>
+    <t>期間FROM</t>
     <rPh sb="0" eb="2">
       <t>ハイシンキカン</t>
     </rPh>
@@ -384,8 +374,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -438,7 +430,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="31">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -453,6 +445,7 @@
     <cellStyle name="ハイパーリンク" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -468,6 +461,7 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="30" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -907,7 +901,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1023,7 +1017,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>18</v>
@@ -1031,14 +1025,14 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>18</v>
@@ -1046,41 +1040,41 @@
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -1097,56 +1091,52 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:6">
       <c r="A17" s="10" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="F17" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G17" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:6">
       <c r="A18" s="2">
         <v>1</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>32</v>
       </c>
       <c r="D18" s="12">
         <v>41624</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12">
+      <c r="E18" s="12">
         <v>41624.166666666664</v>
       </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[強制DM] [delete data] scinario_22 newのappseed修正02
</commit_message>
<xml_diff>
--- a/app/seeds/news.xlsx
+++ b/app/seeds/news.xlsx
@@ -257,13 +257,13 @@
   </si>
   <si>
     <t>期間FROM</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>期間FROM</t>
     <rPh sb="0" eb="2">
       <t>ハイシンキカン</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>期間TO</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -901,7 +901,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1102,10 +1102,10 @@
         <v>40</v>
       </c>
       <c r="D17" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>41</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
[強制DM] [delete data] scinario_22 newのappseed修正03
</commit_message>
<xml_diff>
--- a/app/seeds/news.xlsx
+++ b/app/seeds/news.xlsx
@@ -374,8 +374,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -430,7 +434,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="35">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -446,6 +450,8 @@
     <cellStyle name="ハイパーリンク" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -462,6 +468,8 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="34" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -901,7 +909,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
[強制DM] [add schema] scinario_16
</commit_message>
<xml_diff>
--- a/app/seeds/news.xlsx
+++ b/app/seeds/news.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="22200" windowHeight="14920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="お知らせ" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>コレクション定義</t>
     <phoneticPr fontId="1"/>
@@ -170,12 +170,69 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>news_start_at</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>news_end_at</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>お知らせ期間FROM</t>
     <rPh sb="1" eb="2">
       <t>シ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>お知らせ期間TO</t>
+    <rPh sb="1" eb="2">
+      <t>シ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>お知らせ期間FROM</t>
+    <rPh sb="1" eb="2">
+      <t>シ</t>
+    </rPh>
     <rPh sb="4" eb="6">
       <t>ハイシンキカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>お知らせ期間TO</t>
+    <rPh sb="1" eb="2">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ハイシンキカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>news_outline</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>news_detail</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>お知らせアウトライン</t>
+    <rPh sb="1" eb="2">
+      <t>シ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>お知らせ詳細</t>
+    <rPh sb="1" eb="2">
+      <t>シ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ショウサイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -198,81 +255,19 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-      </rPr>
-      <t>本日22:00よりサーバーメンテナンスが行われます。</t>
-    </r>
-    <rPh sb="0" eb="2">
-      <t>ホンジツ</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>オコナ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2013/12/16 22:00 - 4:00 にサーバメンテナンスが行われます。</t>
-    <rPh sb="35" eb="36">
-      <t>オコナ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>outline</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>detail</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>start_at</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>end_at</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>アウトライン</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>詳細</t>
-    <rPh sb="0" eb="2">
+    <t>お知らせ詳細</t>
+    <rPh sb="1" eb="3">
+      <t>▽シ*r</t>
+    </rPh>
+    <rPh sb="4" eb="6">
       <t>▽ショウサイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>期間FROM</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>期間TO</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>詳細</t>
-    <rPh sb="0" eb="2">
-      <t>ショウサイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>期間FROM</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>期間TO</t>
-    <rPh sb="0" eb="2">
-      <t>ハイシンキカン</t>
+    <t>お知らせアウトライン</t>
+    <rPh sb="1" eb="3">
+      <t>▽シ*r</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -281,7 +276,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -314,19 +309,6 @@
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Hiragino Kaku Gothic Pro"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
     </font>
   </fonts>
   <fills count="4">
@@ -384,7 +366,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -404,12 +386,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -429,10 +407,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="19">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -442,8 +418,6 @@
     <cellStyle name="ハイパーリンク" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -454,8 +428,6 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="22" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -895,7 +867,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1019,7 +991,7 @@
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="7"/>
@@ -1034,41 +1006,41 @@
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="8" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="6" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -1090,53 +1062,32 @@
         <v>26</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="2">
-        <v>1</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="12">
-        <v>41624</v>
-      </c>
-      <c r="E18" s="12">
-        <v>41624.166666666664</v>
-      </c>
-      <c r="F18" s="12">
-        <v>41624.25</v>
-      </c>
-      <c r="G18" s="2"/>
-    </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[強制DM] [add schema] scinario_16_03
</commit_message>
<xml_diff>
--- a/app/seeds/news.xlsx
+++ b/app/seeds/news.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="お知らせ" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>コレクション定義</t>
     <phoneticPr fontId="1"/>
@@ -39,6 +39,10 @@
     <t>名前</t>
   </si>
   <si>
+    <t>News</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>表示名</t>
     <rPh sb="0" eb="2">
       <t>ヒョウジ</t>
@@ -49,6 +53,13 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>お知らせマスタ</t>
+    <rPh sb="1" eb="2">
+      <t>シ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>ダウンロード可</t>
     <rPh sb="6" eb="7">
       <t>カ</t>
@@ -105,6 +116,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>news_id</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>整数値</t>
     <rPh sb="0" eb="3">
       <t>セイスウチ</t>
@@ -116,6 +131,17 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>お知らせID</t>
+    <rPh sb="1" eb="2">
+      <t>シ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>outline</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>文字列</t>
     <rPh sb="0" eb="3">
       <t>モジレツ</t>
@@ -123,6 +149,25 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>アウトライン</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>detail</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>詳細</t>
+    <rPh sb="0" eb="2">
+      <t>▽ショウサイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>start_at</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>期間開始</t>
     <rPh sb="0" eb="2">
       <t>キカン</t>
@@ -133,6 +178,14 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>期間FROM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>end_at</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>期間終了</t>
     <rPh sb="0" eb="4">
       <t>キカンシュウリョウ</t>
@@ -140,99 +193,62 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>期間TO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>データ</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>アウトライン</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>詳細</t>
+    <rPh sb="0" eb="2">
+      <t>ショウサイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>期間FROM</t>
+    <rPh sb="0" eb="2">
+      <t>ハイシンキカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>期間TO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>#comment</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>News</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お知らせマスタ</t>
-    <rPh sb="1" eb="2">
-      <t>シ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>news_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お知らせID</t>
-    <rPh sb="1" eb="2">
-      <t>シ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>news_start_at</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>news_end_at</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お知らせ期間FROM</t>
-    <rPh sb="1" eb="2">
-      <t>シ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お知らせ期間TO</t>
-    <rPh sb="1" eb="2">
-      <t>シ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お知らせ期間FROM</t>
-    <rPh sb="1" eb="2">
-      <t>シ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ハイシンキカン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お知らせ期間TO</t>
-    <rPh sb="1" eb="2">
-      <t>シ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ハイシンキカン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>news_outline</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>news_detail</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お知らせアウトライン</t>
-    <rPh sb="1" eb="2">
-      <t>シ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お知らせ詳細</t>
-    <rPh sb="1" eb="2">
-      <t>シ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ショウサイ</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+      </rPr>
+      <t>本日22:00よりサーバーメンテナンスが行われます。</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>ホンジツ</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>オコナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2013/12/16 22:00 - 4:00 にサーバメンテナンスが行われます。</t>
+    <rPh sb="35" eb="36">
+      <t>オコナ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -247,27 +263,6 @@
     </rPh>
     <rPh sb="19" eb="21">
       <t>シュトク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>◯</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お知らせ詳細</t>
-    <rPh sb="1" eb="3">
-      <t>▽シ*r</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>▽ショウサイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お知らせアウトライン</t>
-    <rPh sb="1" eb="3">
-      <t>▽シ*r</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -293,22 +288,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="12"/>
-      <color theme="10"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <color theme="1"/>
+      <name val="Hiragino Kaku Gothic Pro"/>
       <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="12"/>
-      <color theme="11"/>
+      <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
+      <family val="3"/>
       <charset val="128"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -366,28 +356,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -407,35 +379,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="19">
-    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="ハイパーリンク" xfId="17" builtinId="8" hidden="1"/>
+  <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="表示済みのハイパーリンク" xfId="18" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -456,13 +407,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="角丸四角形吹き出し 2"/>
+        <xdr:cNvPr id="2" name="角丸四角形吹き出し 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7480300" y="0"/>
-          <a:ext cx="4622800" cy="1511300"/>
+          <a:off x="7289800" y="0"/>
+          <a:ext cx="3568700" cy="1511300"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst/>
@@ -864,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E24" sqref="E24:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -875,7 +826,7 @@
     <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.33203125" customWidth="1"/>
     <col min="3" max="3" width="32.1640625" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="28.5" customWidth="1"/>
     <col min="6" max="6" width="32.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" customWidth="1"/>
@@ -905,28 +856,28 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="4"/>
     </row>
@@ -936,45 +887,45 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="6" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F10" s="6">
         <v>1</v>
@@ -983,30 +934,30 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="6" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="6" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -1016,10 +967,10 @@
         <v>27</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="8" t="s">
@@ -1030,17 +981,17 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -1054,46 +1005,60 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="10" t="s">
-        <v>26</v>
-      </c>
       <c r="B17" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="E17" s="10" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="2">
+        <v>1</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="12">
+        <v>41624</v>
+      </c>
+      <c r="E18" s="12">
+        <v>41624.166666666664</v>
+      </c>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
[強制DM] [add field] scinario_17_02
</commit_message>
<xml_diff>
--- a/app/seeds/news.xlsx
+++ b/app/seeds/news.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>コレクション定義</t>
     <phoneticPr fontId="1"/>
@@ -266,12 +266,28 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>title</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイトル</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイトル</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイトル</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -299,6 +315,24 @@
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -356,8 +390,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -382,8 +420,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -815,10 +857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:E25"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -997,68 +1039,92 @@
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="5"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="A15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="10" t="s">
+    <row r="18" spans="1:7">
+      <c r="A18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B18" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C18" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D18" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F18" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="2">
+    <row r="19" spans="1:7">
+      <c r="A19" s="2">
         <v>1</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B19" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C19" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D19" s="12">
         <v>41624</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E19" s="12">
         <v>41624.166666666664</v>
       </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" t="s">
+      <c r="F19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="A21" t="s">
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
[強制DM] [add field] scinario_17_01
</commit_message>
<xml_diff>
--- a/app/seeds/news.xlsx
+++ b/app/seeds/news.xlsx
@@ -856,7 +856,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="13" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1039,7 +1039,7 @@
         <v>43</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>20</v>

</xml_diff>